<commit_message>
impl screenshot into extentreport
</commit_message>
<xml_diff>
--- a/BenchMark/src/test/java/testdata/ports.xlsx
+++ b/BenchMark/src/test/java/testdata/ports.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Name of the Port</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>Port's Label for the result</t>
+  </si>
+  <si>
+    <t>PORT OF DEPARTURE</t>
   </si>
 </sst>
 </file>
@@ -383,16 +386,16 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.109375" customWidth="1"/>
-    <col min="2" max="2" width="21.5546875" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -400,15 +403,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>

</xml_diff>